<commit_message>
Se termino la api de Academic, Falta correccion de poner usuario a cada reporte.
</commit_message>
<xml_diff>
--- a/ARCHIVOS/academicapi.xlsx
+++ b/ARCHIVOS/academicapi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B13FE4C7-887A-4B3E-A7D2-06309325BF10}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7BD87498-43F6-4AAB-9E04-0D999FAE4CB9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="131">
   <si>
     <t>usuarios</t>
   </si>
@@ -46,9 +46,6 @@
     <t>DESCRIPTION</t>
   </si>
   <si>
-    <t>usuario,contraseña,nombre,apellidoP,apellidoM,correo,curriculum,foto,correo,permisos</t>
-  </si>
-  <si>
     <t>usuario</t>
   </si>
   <si>
@@ -350,13 +347,79 @@
   </si>
   <si>
     <t>Bora un reporte4 de la bd</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Línea innovadora de investigación aplicada al desarrollo tecnológico</t>
+  </si>
+  <si>
+    <t>Producción académica</t>
+  </si>
+  <si>
+    <t>Proyectos de investigación aplicada y proyectos tecnológicos</t>
+  </si>
+  <si>
+    <t>Dirección Individualizada</t>
+  </si>
+  <si>
+    <t>Estadía en empresas</t>
+  </si>
+  <si>
+    <t>Subtipo</t>
+  </si>
+  <si>
+    <t>Artículos de difusión y divulgación</t>
+  </si>
+  <si>
+    <t>Artículo arbitrado</t>
+  </si>
+  <si>
+    <t>Artículo en revista indexada</t>
+  </si>
+  <si>
+    <t>Capítulo del libro</t>
+  </si>
+  <si>
+    <t>Informe técnico</t>
+  </si>
+  <si>
+    <t>Libro</t>
+  </si>
+  <si>
+    <t>Manuales de operación</t>
+  </si>
+  <si>
+    <t>Memorias</t>
+  </si>
+  <si>
+    <t>Productividad innovadora</t>
+  </si>
+  <si>
+    <t>Prototipo</t>
+  </si>
+  <si>
+    <t>r1</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>r3</t>
+  </si>
+  <si>
+    <t>r4</t>
+  </si>
+  <si>
+    <t>usuario,contraseña,permisos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -378,6 +441,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -417,13 +486,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Énfasis1" xfId="2" builtinId="30"/>
@@ -709,7 +779,7 @@
   <dimension ref="A1:J72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,37 +792,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="A1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -760,161 +838,232 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="G5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="s">
-        <v>23</v>
-      </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>31</v>
       </c>
-      <c r="E10" t="s">
-        <v>32</v>
+      <c r="G10" t="s">
+        <v>126</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A12" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="G12" t="s">
+        <v>126</v>
+      </c>
+      <c r="H12">
         <v>3</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="I12" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G13" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>1</v>
       </c>
@@ -922,76 +1071,129 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <v>5</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15">
+        <v>6</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="G16" t="s">
+        <v>128</v>
+      </c>
+      <c r="H16">
+        <v>7</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>127</v>
+      </c>
+      <c r="H17">
+        <v>8</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="G18" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18">
+        <v>9</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H19">
+        <v>10</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -999,110 +1201,110 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" t="s">
         <v>42</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="B21" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>12</v>
-      </c>
-      <c r="D21" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E22" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" t="s">
-        <v>42</v>
-      </c>
-      <c r="E23" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>33</v>
-      </c>
-      <c r="D24" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" t="s">
+    <row r="26" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-    </row>
-    <row r="27" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1110,106 +1312,106 @@
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" t="s">
         <v>60</v>
       </c>
-      <c r="D28" t="s">
-        <v>51</v>
-      </c>
-      <c r="E28" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>52</v>
-      </c>
-      <c r="E29" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>11</v>
-      </c>
-      <c r="B30" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
-        <v>12</v>
-      </c>
-      <c r="D30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>18</v>
-      </c>
-      <c r="B31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" t="s">
-        <v>61</v>
-      </c>
-      <c r="D31" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" t="s">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>32</v>
+      </c>
+      <c r="D32" t="s">
+        <v>30</v>
+      </c>
+      <c r="E32" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" t="s">
+    <row r="34" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
+      <c r="A35" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1221,106 +1423,106 @@
         <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
         <v>11</v>
       </c>
-      <c r="B37" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" t="s">
-        <v>12</v>
-      </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
         <v>11</v>
       </c>
-      <c r="B38" t="s">
-        <v>36</v>
-      </c>
-      <c r="C38" t="s">
-        <v>12</v>
-      </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E38" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" t="s">
         <v>62</v>
       </c>
-      <c r="D39" t="s">
-        <v>63</v>
-      </c>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>29</v>
+      </c>
+      <c r="B40" t="s">
+        <v>2</v>
+      </c>
+      <c r="C40" t="s">
+        <v>32</v>
+      </c>
+      <c r="D40" t="s">
         <v>30</v>
       </c>
-      <c r="B40" t="s">
-        <v>2</v>
-      </c>
-      <c r="C40" t="s">
-        <v>33</v>
-      </c>
-      <c r="D40" t="s">
-        <v>31</v>
-      </c>
       <c r="E40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
     </row>
     <row r="43" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="E43" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1332,106 +1534,106 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" t="s">
+        <v>2</v>
+      </c>
+      <c r="C45" t="s">
         <v>11</v>
       </c>
-      <c r="B45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s">
-        <v>12</v>
-      </c>
       <c r="D45" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" t="s">
         <v>11</v>
       </c>
-      <c r="B46" t="s">
-        <v>36</v>
-      </c>
-      <c r="C46" t="s">
-        <v>12</v>
-      </c>
       <c r="D46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E46" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E47" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>29</v>
+      </c>
+      <c r="B48" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" t="s">
+        <v>32</v>
+      </c>
+      <c r="D48" t="s">
         <v>30</v>
       </c>
-      <c r="B48" t="s">
-        <v>2</v>
-      </c>
-      <c r="C48" t="s">
-        <v>33</v>
-      </c>
-      <c r="D48" t="s">
-        <v>31</v>
-      </c>
       <c r="E48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50" s="2"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2"/>
+      <c r="A50" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50" s="4"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B51" s="3" t="s">
+      <c r="B51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C51" s="3" t="s">
+      <c r="C51" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1443,106 +1645,106 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" t="s">
+        <v>2</v>
+      </c>
+      <c r="C53" t="s">
         <v>11</v>
       </c>
-      <c r="B53" t="s">
-        <v>2</v>
-      </c>
-      <c r="C53" t="s">
-        <v>12</v>
-      </c>
       <c r="D53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E53" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>10</v>
+      </c>
+      <c r="B54" t="s">
+        <v>35</v>
+      </c>
+      <c r="C54" t="s">
         <v>11</v>
       </c>
-      <c r="B54" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" t="s">
-        <v>12</v>
-      </c>
       <c r="D54" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E55" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>32</v>
+      </c>
+      <c r="D56" t="s">
         <v>30</v>
       </c>
-      <c r="B56" t="s">
-        <v>2</v>
-      </c>
-      <c r="C56" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" t="s">
-        <v>31</v>
-      </c>
       <c r="E56" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B58" s="2"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2"/>
-      <c r="E58" s="2"/>
+      <c r="A58" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="A59" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D59" s="3" t="s">
+      <c r="D59" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1554,106 +1756,106 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D60" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E60" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" t="s">
+        <v>2</v>
+      </c>
+      <c r="C61" t="s">
         <v>11</v>
       </c>
-      <c r="B61" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" t="s">
-        <v>12</v>
-      </c>
       <c r="D61" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="C62" t="s">
         <v>11</v>
       </c>
-      <c r="B62" t="s">
-        <v>36</v>
-      </c>
-      <c r="C62" t="s">
-        <v>12</v>
-      </c>
       <c r="D62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E62" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B63" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" t="s">
         <v>92</v>
       </c>
-      <c r="D63" t="s">
-        <v>93</v>
-      </c>
       <c r="E63" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>29</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" t="s">
         <v>30</v>
       </c>
-      <c r="B64" t="s">
-        <v>2</v>
-      </c>
-      <c r="C64" t="s">
-        <v>33</v>
-      </c>
-      <c r="D64" t="s">
-        <v>31</v>
-      </c>
       <c r="E64" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
-      <c r="E66" s="2"/>
+      <c r="A66" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+      <c r="A67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="B67" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="C67" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D67" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1665,81 +1867,81 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" t="s">
         <v>11</v>
       </c>
-      <c r="B69" t="s">
-        <v>2</v>
-      </c>
-      <c r="C69" t="s">
-        <v>12</v>
-      </c>
       <c r="D69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E69" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>35</v>
+      </c>
+      <c r="C70" t="s">
         <v>11</v>
       </c>
-      <c r="B70" t="s">
-        <v>36</v>
-      </c>
-      <c r="C70" t="s">
-        <v>12</v>
-      </c>
       <c r="D70" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E70" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D71" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" t="s">
         <v>30</v>
       </c>
-      <c r="B72" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" t="s">
-        <v>33</v>
-      </c>
-      <c r="D72" t="s">
-        <v>31</v>
-      </c>
       <c r="E72" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1755,5 +1957,6 @@
     <mergeCell ref="A34:E34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se corrigio error en bd.
</commit_message>
<xml_diff>
--- a/ARCHIVOS/academicapi.xlsx
+++ b/ARCHIVOS/academicapi.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7BD87498-43F6-4AAB-9E04-0D999FAE4CB9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9A78ACB3-7766-4C3C-B77A-B4391B44A8B5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -256,9 +256,6 @@
     <t>tipo,autores,fecha,nombre,linea,subtipo,isbn,nom_libro</t>
   </si>
   <si>
-    <t>autores,fecha,nombre,linea,isbn,nom_libro</t>
-  </si>
-  <si>
     <t>Reporte_3 /reporte3/</t>
   </si>
   <si>
@@ -413,6 +410,9 @@
   </si>
   <si>
     <t>usuario,contraseña,permisos</t>
+  </si>
+  <si>
+    <t>autores,fecha,nombre,linea,icbn,nom_libro</t>
   </si>
 </sst>
 </file>
@@ -778,8 +778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,7 +802,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -850,7 +850,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -873,7 +873,7 @@
         <v>3</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -893,13 +893,13 @@
         <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -919,13 +919,13 @@
         <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -979,7 +979,7 @@
         <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -999,24 +999,24 @@
         <v>31</v>
       </c>
       <c r="G10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H11">
         <v>2</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1028,13 +1028,13 @@
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="G12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H12">
         <v>3</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1054,13 +1054,13 @@
         <v>7</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13">
         <v>4</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1083,7 +1083,7 @@
         <v>5</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1103,13 +1103,13 @@
         <v>28</v>
       </c>
       <c r="G15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H15">
         <v>6</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1129,24 +1129,24 @@
         <v>34</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H16">
         <v>7</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17">
         <v>8</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1158,13 +1158,13 @@
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H18">
         <v>9</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1184,13 +1184,13 @@
         <v>7</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1585,7 +1585,7 @@
         <v>35</v>
       </c>
       <c r="C47" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="D47" t="s">
         <v>70</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="50" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1645,13 +1645,13 @@
         <v>2</v>
       </c>
       <c r="C52" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E52" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1665,10 +1665,10 @@
         <v>11</v>
       </c>
       <c r="D53" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1682,10 +1682,10 @@
         <v>11</v>
       </c>
       <c r="D54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1696,13 +1696,13 @@
         <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1719,12 +1719,12 @@
         <v>30</v>
       </c>
       <c r="E56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1756,13 +1756,13 @@
         <v>2</v>
       </c>
       <c r="C60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D60" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E60" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1776,10 +1776,10 @@
         <v>11</v>
       </c>
       <c r="D61" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E61" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,10 +1793,10 @@
         <v>11</v>
       </c>
       <c r="D62" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,13 +1807,13 @@
         <v>35</v>
       </c>
       <c r="C63" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63" t="s">
         <v>91</v>
       </c>
-      <c r="D63" t="s">
-        <v>92</v>
-      </c>
       <c r="E63" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1830,12 +1830,12 @@
         <v>30</v>
       </c>
       <c r="E64" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
@@ -1867,13 +1867,13 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D68" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1887,10 +1887,10 @@
         <v>11</v>
       </c>
       <c r="D69" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E69" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1904,10 +1904,10 @@
         <v>11</v>
       </c>
       <c r="D70" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E70" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1918,13 +1918,13 @@
         <v>35</v>
       </c>
       <c r="C71" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1941,7 +1941,7 @@
         <v>30</v>
       </c>
       <c r="E72" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>